<commit_message>
modified:   Portfolio Activity/Documentation/Classify the assets connected to a home network/classify-the-assets-connected-to-a-home-network.md Added
</commit_message>
<xml_diff>
--- a/Portfolio Activity/Documentation/Classify the assets connected to a home network/Home-asset-inventory.xlsx
+++ b/Portfolio Activity/Documentation/Classify the assets connected to a home network/Home-asset-inventory.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Portfolio\projects\Coursera-Cybersecurity\Portfolio Activity\Documentation\Classify the assets connected to a home network\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">Sheet1!$A$1:$G$7</definedName>
-    <definedName hidden="1" localSheetId="0" name="Z_C86149E5_7B16_463F_895B_F05A12B3AD69_.wvu.FilterData">Sheet1!$A$1:$E$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$7</definedName>
+    <definedName name="Z_C86149E5_7B16_463F_895B_F05A12B3AD69_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$E$7</definedName>
   </definedNames>
-  <calcPr/>
+  <calcPr calcId="0"/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{C86149E5-7B16-463F-895B-F05A12B3AD69}" name="Filter 1"/>
+    <customWorkbookView name="Filter 1" guid="{C86149E5-7B16-463F-895B-F05A12B3AD69}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
   <si>
     <t>Asset</t>
   </si>
@@ -104,89 +113,99 @@
   </si>
   <si>
     <t>Anyone</t>
+  </si>
+  <si>
+    <t>External hard drive</t>
+  </si>
+  <si>
+    <t>Printer</t>
+  </si>
+  <si>
+    <t>Webcam</t>
+  </si>
+  <si>
+    <t>Has a 1080 pixel, connected to Desktop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="12">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <i/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="12.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
+      <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -202,43 +221,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
   <borders count="5">
-    <border/>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -247,99 +241,123 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="5" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -529,33 +547,36 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="5.88"/>
-    <col customWidth="1" min="2" max="2" width="17.5"/>
-    <col customWidth="1" min="3" max="3" width="18.63"/>
-    <col customWidth="1" min="4" max="4" width="27.63"/>
-    <col customWidth="1" min="5" max="5" width="19.5"/>
-    <col customWidth="1" min="6" max="6" width="35.0"/>
-    <col customWidth="1" min="7" max="7" width="13.5"/>
-    <col customWidth="1" min="10" max="10" width="20.88"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="35" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22.5" customHeight="1">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -580,9 +601,9 @@
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>6</v>
@@ -611,9 +632,9 @@
       </c>
       <c r="K2" s="5"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>14</v>
@@ -642,9 +663,9 @@
       </c>
       <c r="K3" s="5"/>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" ht="30.75" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>20</v>
@@ -673,16 +694,28 @@
       </c>
       <c r="K4" s="5"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="H5" s="5"/>
       <c r="I5" s="12" t="s">
         <v>24</v>
@@ -692,16 +725,28 @@
       </c>
       <c r="K5" s="5"/>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
-        <v>5.0</v>
-      </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="H6" s="5"/>
       <c r="I6" s="12" t="s">
         <v>27</v>
@@ -711,68 +756,81 @@
       </c>
       <c r="K6" s="5"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
-        <v>6.0</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="14"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>24</v>
+      </c>
       <c r="H7" s="5"/>
       <c r="K7" s="5"/>
     </row>
-    <row r="10">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="18"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="18"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="21"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="18"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="18"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="18"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
+    <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A10" s="14"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="14"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
+    </row>
+    <row r="12" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A12" s="14"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A13" s="14"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A14" s="14"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+    </row>
+    <row r="15" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="14"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
     </row>
   </sheetData>
-  <autoFilter ref="$A$1:$G$7"/>
+  <autoFilter ref="A1:G7"/>
   <customSheetViews>
     <customSheetView guid="{C86149E5-7B16-463F-895B-F05A12B3AD69}" filter="1" showAutoFilter="1">
-      <autoFilter ref="$A$1:$E$7"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:E7"/>
     </customSheetView>
   </customSheetViews>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>